<commit_message>
0.2.2 Added predetermined discount option
Added predetermined discount option
</commit_message>
<xml_diff>
--- a/excels/materiales/01Agregados.xlsx
+++ b/excels/materiales/01Agregados.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\COTOCO\excels\materiales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuelziga/Desktop/materiales/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="456" windowWidth="22716" windowHeight="13464"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="22720" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -75,15 +75,25 @@
   </si>
   <si>
     <t>metro3</t>
+  </si>
+  <si>
+    <t>product_discount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -531,51 +541,52 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -601,7 +612,6 @@
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
@@ -618,6 +628,7 @@
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -922,27 +933,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -964,18 +976,23 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1001</v>
+      </c>
       <c r="B2" s="2">
         <v>1001</v>
       </c>
@@ -1003,9 +1020,14 @@
       <c r="J2" s="2">
         <v>1</v>
       </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1002</v>
+      </c>
       <c r="B3" s="2">
         <v>1002</v>
       </c>
@@ -1033,9 +1055,14 @@
       <c r="J3" s="2">
         <v>1</v>
       </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1003</v>
+      </c>
       <c r="B4" s="2">
         <v>1003</v>
       </c>
@@ -1062,6 +1089,9 @@
       </c>
       <c r="J4" s="2">
         <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.2.3 added excel products
added excel products
</commit_message>
<xml_diff>
--- a/excels/materiales/01Agregados.xlsx
+++ b/excels/materiales/01Agregados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuelziga/Desktop/materiales/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuelziga/GITHUB/COTOCO/excels/materiales/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -78,15 +78,34 @@
   </si>
   <si>
     <t>product_discount</t>
+  </si>
+  <si>
+    <t>Product_discount</t>
+  </si>
+  <si>
+    <t>15486.73</t>
+  </si>
+  <si>
+    <t>1734.51</t>
+  </si>
+  <si>
+    <t>13805.31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
+  <fonts count="22" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -242,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +439,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -541,53 +566,58 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -933,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,10 +981,10 @@
     <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -988,109 +1018,121 @@
       <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="L1" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>1001</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>1001</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2">
-        <v>15486.73</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="5">
         <v>13</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="5">
         <v>1</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="7">
         <v>0</v>
       </c>
+      <c r="L2" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>1002</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>1002</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2">
-        <v>1734.51</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="5">
         <v>13</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="5">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="7">
         <v>0</v>
       </c>
+      <c r="L3" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>1003</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>1003</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
-        <v>13805.31</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="5">
         <v>13</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.2.5 Minor Fixes and improvements
Minor Fixes and improvements
</commit_message>
<xml_diff>
--- a/excels/materiales/01Agregados.xlsx
+++ b/excels/materiales/01Agregados.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuelziga/GITHUB/COTOCO/excels/materiales/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuelziga/GITHUB/COTOCO/materiales/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="22720" windowHeight="13460"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="19320" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>13805.31</t>
+  </si>
+  <si>
+    <t>Iguana piedra drenaje metro</t>
+  </si>
+  <si>
+    <t>Iguana piedra base entreg camion 4x4 m3</t>
+  </si>
+  <si>
+    <t>Agregado lastre de tajo la iguana mt</t>
+  </si>
+  <si>
+    <t>mtr</t>
   </si>
 </sst>
 </file>
@@ -608,16 +620,42 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -719,7 +757,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -754,7 +792,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -963,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E5" sqref="A5:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,14 +1012,13 @@
     <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="10" customWidth="1"/>
+    <col min="8" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -997,13 +1034,13 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1022,7 +1059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1001</v>
       </c>
@@ -1035,13 +1072,13 @@
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="5">
@@ -1053,14 +1090,14 @@
       <c r="J2" s="5">
         <v>1</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>0</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1002</v>
       </c>
@@ -1073,13 +1110,13 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="5">
@@ -1091,14 +1128,14 @@
       <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>0</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1003</v>
       </c>
@@ -1111,13 +1148,13 @@
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="5">
@@ -1129,10 +1166,124 @@
       <c r="J4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>1004</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1004</v>
+      </c>
+      <c r="C5" s="14">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="16">
+        <v>15000</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="14">
+        <v>13</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <v>1</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>1005</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1005</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="16">
+        <v>16778.759999999998</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="14">
+        <v>13</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
+        <v>1</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>1006</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1006</v>
+      </c>
+      <c r="C7" s="14">
+        <v>6</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="16">
+        <v>16000</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="14">
+        <v>13</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
+        <v>1</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1141,6 +1292,6 @@
     <sortCondition ref="C2:C4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>